<commit_message>
fully functional charging station
</commit_message>
<xml_diff>
--- a/output/df_schedule.xlsx
+++ b/output/df_schedule.xlsx
@@ -31,292 +31,292 @@
     <t>Others</t>
   </si>
   <si>
+    <t>Audi E-TRON</t>
+  </si>
+  <si>
+    <t>Fiat 500 E</t>
+  </si>
+  <si>
+    <t>Hyundai KONA 39 kWh</t>
+  </si>
+  <si>
+    <t>VW ID.3</t>
+  </si>
+  <si>
+    <t>VW E-UP</t>
+  </si>
+  <si>
+    <t>Polestar 2</t>
+  </si>
+  <si>
+    <t>SKODA ENYAQ 58kWh</t>
+  </si>
+  <si>
+    <t>VW ID.5</t>
+  </si>
+  <si>
+    <t>Opel MOKKA</t>
+  </si>
+  <si>
+    <t>Hyundai KONA 64 kWh</t>
+  </si>
+  <si>
+    <t>VW ID.4</t>
+  </si>
+  <si>
+    <t>Hyundai IONIQ5 77kWh</t>
+  </si>
+  <si>
+    <t>Opel CORSA</t>
+  </si>
+  <si>
+    <t>Hyundai IONIQ5 58kWh</t>
+  </si>
+  <si>
+    <t>Renault ZOE</t>
+  </si>
+  <si>
+    <t>Smart FORTWO</t>
+  </si>
+  <si>
+    <t>Tesla MODEL 3</t>
+  </si>
+  <si>
     <t>TESLA MODEL Y</t>
   </si>
   <si>
-    <t>Renault ZOE</t>
-  </si>
-  <si>
     <t>MINI Cooper SE</t>
   </si>
   <si>
-    <t>Audi E-TRON</t>
-  </si>
-  <si>
-    <t>Fiat 500 E</t>
-  </si>
-  <si>
-    <t>VW ID.4</t>
-  </si>
-  <si>
-    <t>Smart FORTWO</t>
+    <t>Audi Q4</t>
   </si>
   <si>
     <t>SKODA ENYAQ 77kWh</t>
   </si>
   <si>
-    <t>VW E-UP</t>
-  </si>
-  <si>
-    <t>Hyundai KONA 39 kWh</t>
-  </si>
-  <si>
-    <t>Renault TWINGO</t>
-  </si>
-  <si>
-    <t>Hyundai IONIQ5 58kWh</t>
-  </si>
-  <si>
-    <t>Opel MOKKA</t>
-  </si>
-  <si>
-    <t>VW ID.5</t>
-  </si>
-  <si>
-    <t>Tesla MODEL 3</t>
-  </si>
-  <si>
-    <t>KIA EV6</t>
-  </si>
-  <si>
-    <t>Opel CORSA</t>
-  </si>
-  <si>
-    <t>Polestar 2</t>
-  </si>
-  <si>
-    <t>Hyundai IONIQ5 77kWh</t>
-  </si>
-  <si>
-    <t>Audi Q4</t>
-  </si>
-  <si>
-    <t>VW ID.3</t>
-  </si>
-  <si>
-    <t>Peugeot 208</t>
-  </si>
-  <si>
-    <t>2023-10-01 06:26</t>
-  </si>
-  <si>
-    <t>2023-10-01 06:17</t>
-  </si>
-  <si>
-    <t>2023-10-01 05:35</t>
-  </si>
-  <si>
-    <t>2023-10-01 06:14</t>
-  </si>
-  <si>
-    <t>2023-10-01 06:04</t>
-  </si>
-  <si>
-    <t>2023-10-01 11:45</t>
-  </si>
-  <si>
-    <t>2023-10-01 11:50</t>
-  </si>
-  <si>
-    <t>2023-10-01 12:53</t>
-  </si>
-  <si>
-    <t>2023-10-01 12:20</t>
-  </si>
-  <si>
-    <t>2023-10-01 11:28</t>
-  </si>
-  <si>
-    <t>2023-10-01 18:47</t>
-  </si>
-  <si>
-    <t>2023-10-01 16:57</t>
-  </si>
-  <si>
-    <t>2023-10-01 18:28</t>
-  </si>
-  <si>
-    <t>2023-10-01 17:51</t>
-  </si>
-  <si>
-    <t>2023-10-01 18:55</t>
-  </si>
-  <si>
-    <t>2023-10-02 05:13</t>
-  </si>
-  <si>
-    <t>2023-10-02 05:55</t>
-  </si>
-  <si>
-    <t>2023-10-02 05:14</t>
-  </si>
-  <si>
-    <t>2023-10-02 06:13</t>
-  </si>
-  <si>
-    <t>2023-10-02 12:03</t>
-  </si>
-  <si>
-    <t>2023-10-02 13:03</t>
-  </si>
-  <si>
-    <t>2023-10-02 11:39</t>
-  </si>
-  <si>
-    <t>2023-10-02 11:31</t>
+    <t>2023-10-01 08:36</t>
+  </si>
+  <si>
+    <t>2023-10-01 08:31</t>
+  </si>
+  <si>
+    <t>2023-10-01 07:47</t>
+  </si>
+  <si>
+    <t>2023-10-01 07:36</t>
+  </si>
+  <si>
+    <t>2023-10-01 08:02</t>
+  </si>
+  <si>
+    <t>2023-10-01 12:37</t>
+  </si>
+  <si>
+    <t>2023-10-01 12:13</t>
+  </si>
+  <si>
+    <t>2023-10-01 12:19</t>
+  </si>
+  <si>
+    <t>2023-10-01 12:11</t>
+  </si>
+  <si>
+    <t>2023-10-01 12:43</t>
+  </si>
+  <si>
+    <t>2023-10-01 15:30</t>
+  </si>
+  <si>
+    <t>2023-10-01 15:32</t>
+  </si>
+  <si>
+    <t>2023-10-01 16:07</t>
+  </si>
+  <si>
+    <t>2023-10-01 15:54</t>
+  </si>
+  <si>
+    <t>2023-10-01 15:34</t>
+  </si>
+  <si>
+    <t>2023-10-02 08:09</t>
+  </si>
+  <si>
+    <t>2023-10-02 07:39</t>
+  </si>
+  <si>
+    <t>2023-10-02 07:47</t>
+  </si>
+  <si>
+    <t>2023-10-02 09:02</t>
+  </si>
+  <si>
+    <t>2023-10-02 08:33</t>
+  </si>
+  <si>
+    <t>2023-10-02 12:28</t>
+  </si>
+  <si>
+    <t>2023-10-02 12:12</t>
+  </si>
+  <si>
+    <t>2023-10-02 12:09</t>
   </si>
   <si>
     <t>2023-10-02 12:22</t>
   </si>
   <si>
-    <t>2023-10-02 17:27</t>
-  </si>
-  <si>
-    <t>2023-10-02 18:22</t>
-  </si>
-  <si>
-    <t>2023-10-02 18:53</t>
-  </si>
-  <si>
-    <t>2023-10-02 18:20</t>
-  </si>
-  <si>
-    <t>2023-10-02 17:42</t>
-  </si>
-  <si>
-    <t>2023-10-03 06:32</t>
-  </si>
-  <si>
-    <t>2023-10-03 05:29</t>
-  </si>
-  <si>
-    <t>2023-10-03 06:01</t>
-  </si>
-  <si>
-    <t>2023-10-03 05:35</t>
-  </si>
-  <si>
-    <t>2023-10-03 06:21</t>
-  </si>
-  <si>
-    <t>2023-10-03 13:10</t>
+    <t>2023-10-02 12:02</t>
+  </si>
+  <si>
+    <t>2023-10-02 16:52</t>
+  </si>
+  <si>
+    <t>2023-10-02 15:17</t>
+  </si>
+  <si>
+    <t>2023-10-02 16:11</t>
+  </si>
+  <si>
+    <t>2023-10-02 15:38</t>
+  </si>
+  <si>
+    <t>2023-10-02 16:26</t>
+  </si>
+  <si>
+    <t>2023-10-03 07:30</t>
+  </si>
+  <si>
+    <t>2023-10-03 08:30</t>
+  </si>
+  <si>
+    <t>2023-10-03 06:57</t>
+  </si>
+  <si>
+    <t>2023-10-03 07:51</t>
+  </si>
+  <si>
+    <t>2023-10-03 08:07</t>
+  </si>
+  <si>
+    <t>2023-10-03 11:37</t>
+  </si>
+  <si>
+    <t>2023-10-03 11:18</t>
+  </si>
+  <si>
+    <t>2023-10-03 11:58</t>
   </si>
   <si>
     <t>2023-10-03 11:31</t>
   </si>
   <si>
-    <t>2023-10-03 12:28</t>
-  </si>
-  <si>
-    <t>2023-10-03 11:45</t>
-  </si>
-  <si>
-    <t>2023-10-03 11:50</t>
-  </si>
-  <si>
-    <t>2023-10-03 17:34</t>
-  </si>
-  <si>
-    <t>2023-10-03 18:56</t>
-  </si>
-  <si>
-    <t>2023-10-03 17:41</t>
-  </si>
-  <si>
-    <t>2023-10-03 17:42</t>
-  </si>
-  <si>
-    <t>2023-10-03 17:43</t>
-  </si>
-  <si>
-    <t>2023-10-04 05:09</t>
-  </si>
-  <si>
-    <t>2023-10-04 05:42</t>
-  </si>
-  <si>
-    <t>2023-10-04 05:54</t>
-  </si>
-  <si>
-    <t>2023-10-04 06:20</t>
-  </si>
-  <si>
-    <t>2023-10-04 06:14</t>
-  </si>
-  <si>
-    <t>2023-10-04 11:00</t>
-  </si>
-  <si>
-    <t>2023-10-04 11:58</t>
-  </si>
-  <si>
-    <t>2023-10-04 12:09</t>
-  </si>
-  <si>
-    <t>2023-10-04 11:45</t>
-  </si>
-  <si>
-    <t>2023-10-04 11:29</t>
-  </si>
-  <si>
-    <t>2023-10-04 17:54</t>
-  </si>
-  <si>
-    <t>2023-10-04 17:13</t>
-  </si>
-  <si>
-    <t>2023-10-04 17:39</t>
-  </si>
-  <si>
-    <t>2023-10-04 18:21</t>
-  </si>
-  <si>
-    <t>2023-10-04 18:45</t>
-  </si>
-  <si>
-    <t>2023-10-05 04:58</t>
-  </si>
-  <si>
-    <t>2023-10-05 05:24</t>
-  </si>
-  <si>
-    <t>2023-10-05 05:35</t>
-  </si>
-  <si>
-    <t>2023-10-05 06:33</t>
-  </si>
-  <si>
-    <t>2023-10-05 06:34</t>
-  </si>
-  <si>
-    <t>2023-10-05 12:02</t>
+    <t>2023-10-03 11:47</t>
+  </si>
+  <si>
+    <t>2023-10-03 16:04</t>
+  </si>
+  <si>
+    <t>2023-10-03 15:39</t>
+  </si>
+  <si>
+    <t>2023-10-03 15:32</t>
+  </si>
+  <si>
+    <t>2023-10-03 15:43</t>
+  </si>
+  <si>
+    <t>2023-10-03 16:22</t>
+  </si>
+  <si>
+    <t>2023-10-04 08:34</t>
+  </si>
+  <si>
+    <t>2023-10-04 07:17</t>
+  </si>
+  <si>
+    <t>2023-10-04 06:58</t>
+  </si>
+  <si>
+    <t>2023-10-04 09:27</t>
+  </si>
+  <si>
+    <t>2023-10-04 08:19</t>
+  </si>
+  <si>
+    <t>2023-10-04 12:31</t>
+  </si>
+  <si>
+    <t>2023-10-04 11:34</t>
+  </si>
+  <si>
+    <t>2023-10-04 12:13</t>
+  </si>
+  <si>
+    <t>2023-10-04 12:03</t>
+  </si>
+  <si>
+    <t>2023-10-04 12:21</t>
+  </si>
+  <si>
+    <t>2023-10-04 15:21</t>
+  </si>
+  <si>
+    <t>2023-10-04 15:17</t>
+  </si>
+  <si>
+    <t>2023-10-04 17:00</t>
+  </si>
+  <si>
+    <t>2023-10-04 16:38</t>
+  </si>
+  <si>
+    <t>2023-10-04 16:15</t>
+  </si>
+  <si>
+    <t>2023-10-05 08:03</t>
+  </si>
+  <si>
+    <t>2023-10-05 08:52</t>
+  </si>
+  <si>
+    <t>2023-10-05 08:13</t>
+  </si>
+  <si>
+    <t>2023-10-05 07:55</t>
+  </si>
+  <si>
+    <t>2023-10-05 06:59</t>
+  </si>
+  <si>
+    <t>2023-10-05 12:01</t>
+  </si>
+  <si>
+    <t>2023-10-05 12:28</t>
+  </si>
+  <si>
+    <t>2023-10-05 11:50</t>
   </si>
   <si>
     <t>2023-10-05 11:53</t>
   </si>
   <si>
-    <t>2023-10-05 11:50</t>
-  </si>
-  <si>
-    <t>2023-10-05 11:20</t>
-  </si>
-  <si>
-    <t>2023-10-05 12:04</t>
-  </si>
-  <si>
-    <t>2023-10-05 18:20</t>
-  </si>
-  <si>
-    <t>2023-10-05 18:26</t>
-  </si>
-  <si>
-    <t>2023-10-05 17:27</t>
-  </si>
-  <si>
-    <t>2023-10-05 17:32</t>
-  </si>
-  <si>
-    <t>2023-10-05 17:33</t>
+    <t>2023-10-05 12:07</t>
+  </si>
+  <si>
+    <t>2023-10-05 16:42</t>
+  </si>
+  <si>
+    <t>2023-10-05 16:03</t>
+  </si>
+  <si>
+    <t>2023-10-05 16:14</t>
+  </si>
+  <si>
+    <t>2023-10-05 15:39</t>
+  </si>
+  <si>
+    <t>2023-10-05 16:06</t>
   </si>
 </sst>
 </file>
@@ -699,13 +699,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="D2">
-        <v>0.8500000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -713,27 +713,27 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>0.25</v>
       </c>
       <c r="D3">
-        <v>0.8000000000000002</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>0.4</v>
       </c>
       <c r="D4">
-        <v>0.9500000000000003</v>
+        <v>0.7500000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -741,52 +741,52 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="D5">
-        <v>0.8000000000000002</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6">
-        <v>0.25</v>
+        <v>0.4999999999999999</v>
       </c>
       <c r="D6">
-        <v>0.7000000000000001</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="D7">
-        <v>0.8000000000000002</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D8">
         <v>0.8500000000000002</v>
@@ -797,10 +797,10 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="D9">
         <v>0.8500000000000002</v>
@@ -808,41 +808,41 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="D10">
-        <v>0.65</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="D11">
-        <v>0.7000000000000001</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D12">
         <v>0.8500000000000002</v>
@@ -850,30 +850,30 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="D13">
-        <v>0.8500000000000002</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -881,55 +881,55 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D15">
-        <v>0.7000000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="D16">
-        <v>0.8500000000000002</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="D17">
-        <v>0.9500000000000003</v>
+        <v>0.7500000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="D18">
-        <v>0.8000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -937,60 +937,60 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="D19">
-        <v>0.8500000000000002</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
         <v>44</v>
       </c>
       <c r="C20">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="D20">
-        <v>0.9500000000000003</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
         <v>45</v>
       </c>
       <c r="C21">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="D21">
-        <v>0.7500000000000001</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
         <v>46</v>
       </c>
       <c r="C22">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="D22">
-        <v>0.8500000000000002</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
         <v>47</v>
@@ -1010,99 +1010,99 @@
         <v>48</v>
       </c>
       <c r="C24">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D24">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
         <v>49</v>
       </c>
       <c r="C25">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D25">
-        <v>0.8500000000000002</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B26" t="s">
         <v>50</v>
       </c>
       <c r="C26">
-        <v>0.15</v>
+        <v>0.35</v>
       </c>
       <c r="D26">
-        <v>0.9000000000000002</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
         <v>51</v>
       </c>
       <c r="C27">
-        <v>0.45</v>
+        <v>0.35</v>
       </c>
       <c r="D27">
-        <v>0.8000000000000002</v>
+        <v>0.7500000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
         <v>52</v>
       </c>
       <c r="C28">
-        <v>0.2</v>
+        <v>0.35</v>
       </c>
       <c r="D28">
-        <v>0.9000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
         <v>53</v>
       </c>
       <c r="C29">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="D29">
-        <v>0.7000000000000001</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
         <v>54</v>
       </c>
       <c r="C30">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="D30">
-        <v>0.8500000000000002</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
         <v>55</v>
@@ -1116,7 +1116,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
         <v>56</v>
@@ -1130,58 +1130,58 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B33" t="s">
         <v>57</v>
       </c>
       <c r="C33">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B34" t="s">
         <v>58</v>
       </c>
       <c r="C34">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="D34">
-        <v>0.8500000000000002</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B35" t="s">
         <v>59</v>
       </c>
       <c r="C35">
-        <v>0.05</v>
+        <v>0.35</v>
       </c>
       <c r="D35">
-        <v>0.9000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
         <v>60</v>
       </c>
       <c r="C36">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D36">
-        <v>0.9000000000000002</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1192,10 +1192,10 @@
         <v>61</v>
       </c>
       <c r="C37">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D37">
-        <v>0.7500000000000001</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1206,80 +1206,80 @@
         <v>62</v>
       </c>
       <c r="C38">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="D38">
-        <v>0.8500000000000002</v>
+        <v>0.7500000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B39" t="s">
         <v>63</v>
       </c>
       <c r="C39">
-        <v>0.45</v>
+        <v>0.2</v>
       </c>
       <c r="D39">
-        <v>0.65</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s">
         <v>64</v>
       </c>
       <c r="C40">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="D40">
-        <v>0.9500000000000003</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B41" t="s">
         <v>65</v>
       </c>
       <c r="C41">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D41">
-        <v>0.9500000000000003</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B42" t="s">
         <v>66</v>
       </c>
       <c r="C42">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="D42">
-        <v>0.9000000000000002</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B43" t="s">
         <v>67</v>
       </c>
       <c r="C43">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1293,12 +1293,12 @@
         <v>0.15</v>
       </c>
       <c r="D44">
-        <v>0.8500000000000002</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
         <v>69</v>
@@ -1307,35 +1307,35 @@
         <v>0.3</v>
       </c>
       <c r="D45">
-        <v>0.6</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B46" t="s">
         <v>70</v>
       </c>
       <c r="C46">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="D46">
-        <v>0.8500000000000002</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B47" t="s">
         <v>71</v>
       </c>
       <c r="C47">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="D47">
-        <v>0.9500000000000003</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1346,7 +1346,7 @@
         <v>72</v>
       </c>
       <c r="C48">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D48">
         <v>0.8000000000000002</v>
@@ -1354,69 +1354,69 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B49" t="s">
         <v>73</v>
       </c>
       <c r="C49">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D49">
-        <v>0.7000000000000001</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B50" t="s">
         <v>74</v>
       </c>
       <c r="C50">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D50">
-        <v>0.9500000000000003</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B51" t="s">
         <v>75</v>
       </c>
       <c r="C51">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D51">
-        <v>0.9500000000000003</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B52" t="s">
         <v>76</v>
       </c>
       <c r="C52">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="D52">
-        <v>0.7500000000000001</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B53" t="s">
         <v>77</v>
       </c>
       <c r="C53">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="D53">
         <v>0.8500000000000002</v>
@@ -1424,35 +1424,35 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B54" t="s">
         <v>78</v>
       </c>
       <c r="C54">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D54">
-        <v>0.7500000000000001</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B55" t="s">
         <v>79</v>
       </c>
       <c r="C55">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D55">
-        <v>0.9000000000000002</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B56" t="s">
         <v>80</v>
@@ -1461,18 +1461,18 @@
         <v>0.35</v>
       </c>
       <c r="D56">
-        <v>0.9000000000000002</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B57" t="s">
         <v>81</v>
       </c>
       <c r="C57">
-        <v>0.35</v>
+        <v>0.1</v>
       </c>
       <c r="D57">
         <v>0.8500000000000002</v>
@@ -1480,16 +1480,16 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B58" t="s">
         <v>82</v>
       </c>
       <c r="C58">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="D58">
-        <v>0.7500000000000001</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1500,197 +1500,197 @@
         <v>83</v>
       </c>
       <c r="C59">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="D59">
-        <v>0.8000000000000002</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B60" t="s">
         <v>84</v>
       </c>
       <c r="C60">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D60">
-        <v>0.8000000000000002</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B61" t="s">
         <v>85</v>
       </c>
       <c r="C61">
-        <v>0.45</v>
+        <v>0.3</v>
       </c>
       <c r="D61">
-        <v>0.9500000000000003</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B62" t="s">
         <v>86</v>
       </c>
       <c r="C62">
-        <v>0.45</v>
+        <v>0.1</v>
       </c>
       <c r="D62">
-        <v>0.8000000000000002</v>
+        <v>0.7500000000000001</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B63" t="s">
         <v>87</v>
       </c>
       <c r="C63">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="D63">
-        <v>0.7500000000000001</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B64" t="s">
         <v>88</v>
       </c>
       <c r="C64">
-        <v>0.35</v>
+        <v>0.25</v>
       </c>
       <c r="D64">
-        <v>0.8500000000000002</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B65" t="s">
         <v>89</v>
       </c>
       <c r="C65">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D65">
-        <v>0.7000000000000001</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B66" t="s">
         <v>90</v>
       </c>
       <c r="C66">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="D66">
-        <v>0.7500000000000001</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B67" t="s">
         <v>91</v>
       </c>
       <c r="C67">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D67">
-        <v>0.8500000000000002</v>
+        <v>0.7500000000000001</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B68" t="s">
         <v>92</v>
       </c>
       <c r="C68">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="D68">
-        <v>0.8500000000000002</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B69" t="s">
         <v>93</v>
       </c>
       <c r="C69">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="D69">
-        <v>0.8500000000000002</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B70" t="s">
         <v>94</v>
       </c>
       <c r="C70">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="D70">
-        <v>0.7000000000000001</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B71" t="s">
         <v>95</v>
       </c>
       <c r="C71">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="D71">
-        <v>0.7500000000000001</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B72" t="s">
         <v>96</v>
       </c>
       <c r="C72">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="D72">
-        <v>0.9500000000000003</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B73" t="s">
         <v>97</v>
@@ -1699,49 +1699,49 @@
         <v>0.15</v>
       </c>
       <c r="D73">
-        <v>0.8000000000000002</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B74" t="s">
         <v>98</v>
       </c>
       <c r="C74">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="D74">
-        <v>0.9500000000000003</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B75" t="s">
         <v>99</v>
       </c>
       <c r="C75">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="D75">
-        <v>0.7000000000000001</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B76" t="s">
         <v>100</v>
       </c>
       <c r="C76">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D76">
-        <v>0.9000000000000002</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit for returning later
</commit_message>
<xml_diff>
--- a/output/df_schedule.xlsx
+++ b/output/df_schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="131">
   <si>
     <t>car models</t>
   </si>
@@ -28,382 +28,385 @@
     <t>final SoC</t>
   </si>
   <si>
+    <t>Fiat 500 E</t>
+  </si>
+  <si>
+    <t>Hyundai KONA 39 kWh</t>
+  </si>
+  <si>
+    <t>Tesla MODEL 3</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Smart FORTWO</t>
+  </si>
+  <si>
+    <t>KIA EV6</t>
+  </si>
+  <si>
+    <t>VW E-UP</t>
+  </si>
+  <si>
+    <t>VW ID.3</t>
+  </si>
+  <si>
+    <t>Hyundai KONA 64 kWh</t>
+  </si>
+  <si>
+    <t>Hyundai IONIQ5 77kWh</t>
+  </si>
+  <si>
+    <t>SKODA ENYAQ 77kWh</t>
+  </si>
+  <si>
+    <t>Polestar 2</t>
+  </si>
+  <si>
+    <t>VW ID.4</t>
+  </si>
+  <si>
+    <t>Renault ZOE</t>
+  </si>
+  <si>
+    <t>Audi Q4</t>
+  </si>
+  <si>
+    <t>VW ID.5</t>
+  </si>
+  <si>
+    <t>Opel MOKKA</t>
+  </si>
+  <si>
+    <t>Audi E-TRON</t>
+  </si>
+  <si>
+    <t>TESLA MODEL Y</t>
+  </si>
+  <si>
+    <t>MINI Cooper SE</t>
+  </si>
+  <si>
     <t>Dacia SPRING</t>
   </si>
   <si>
-    <t>Others</t>
-  </si>
-  <si>
-    <t>Audi E-TRON</t>
-  </si>
-  <si>
-    <t>Fiat 500 E</t>
-  </si>
-  <si>
-    <t>Smart FORTWO</t>
-  </si>
-  <si>
-    <t>Renault ZOE</t>
-  </si>
-  <si>
-    <t>Opel CORSA</t>
-  </si>
-  <si>
-    <t>VW E-UP</t>
-  </si>
-  <si>
-    <t>VW ID.3</t>
-  </si>
-  <si>
-    <t>Renault TWINGO</t>
-  </si>
-  <si>
-    <t>VW ID.5</t>
-  </si>
-  <si>
-    <t>TESLA MODEL Y</t>
-  </si>
-  <si>
-    <t>Peugeot 208</t>
-  </si>
-  <si>
-    <t>MINI Cooper SE</t>
-  </si>
-  <si>
-    <t>Tesla MODEL 3</t>
-  </si>
-  <si>
-    <t>SKODA ENYAQ 58kWh</t>
-  </si>
-  <si>
-    <t>SKODA ENYAQ 77kWh</t>
-  </si>
-  <si>
-    <t>Hyundai KONA 64 kWh</t>
-  </si>
-  <si>
-    <t>Audi Q4</t>
-  </si>
-  <si>
-    <t>Hyundai IONIQ5 77kWh</t>
-  </si>
-  <si>
-    <t>Hyundai KONA 39 kWh</t>
-  </si>
-  <si>
     <t>Hyundai IONIQ5 58kWh</t>
   </si>
   <si>
-    <t>VW ID.4</t>
-  </si>
-  <si>
-    <t>2022-02-17 09:03</t>
-  </si>
-  <si>
-    <t>2022-02-17 08:35</t>
-  </si>
-  <si>
-    <t>2022-02-17 09:22</t>
-  </si>
-  <si>
-    <t>2022-02-17 08:21</t>
-  </si>
-  <si>
-    <t>2022-02-17 08:55</t>
-  </si>
-  <si>
-    <t>2022-02-17 07:55</t>
-  </si>
-  <si>
-    <t>2022-02-17 10:33</t>
-  </si>
-  <si>
-    <t>2022-02-17 12:04</t>
-  </si>
-  <si>
-    <t>2022-02-17 12:52</t>
-  </si>
-  <si>
-    <t>2022-02-17 12:01</t>
-  </si>
-  <si>
-    <t>2022-02-17 12:05</t>
-  </si>
-  <si>
-    <t>2022-02-17 11:26</t>
-  </si>
-  <si>
-    <t>2022-02-17 11:52</t>
-  </si>
-  <si>
-    <t>2022-02-17 18:08</t>
-  </si>
-  <si>
-    <t>2022-02-17 16:10</t>
-  </si>
-  <si>
-    <t>2022-02-17 17:52</t>
-  </si>
-  <si>
-    <t>2022-02-17 17:48</t>
-  </si>
-  <si>
-    <t>2022-02-17 20:20</t>
-  </si>
-  <si>
-    <t>2022-02-17 18:32</t>
-  </si>
-  <si>
-    <t>2022-02-17 17:12</t>
-  </si>
-  <si>
-    <t>2022-02-18 08:38</t>
-  </si>
-  <si>
-    <t>2022-02-18 08:52</t>
-  </si>
-  <si>
-    <t>2022-02-18 07:31</t>
-  </si>
-  <si>
-    <t>2022-02-18 08:50</t>
-  </si>
-  <si>
-    <t>2022-02-18 07:20</t>
-  </si>
-  <si>
-    <t>2022-02-18 06:46</t>
-  </si>
-  <si>
-    <t>2022-02-18 07:54</t>
-  </si>
-  <si>
-    <t>2022-02-18 09:38</t>
-  </si>
-  <si>
-    <t>2022-02-18 09:56</t>
-  </si>
-  <si>
-    <t>2022-02-18 11:22</t>
-  </si>
-  <si>
-    <t>2022-02-18 12:28</t>
-  </si>
-  <si>
-    <t>2022-02-18 12:21</t>
-  </si>
-  <si>
-    <t>2022-02-18 10:24</t>
-  </si>
-  <si>
-    <t>2022-02-18 12:48</t>
-  </si>
-  <si>
-    <t>2022-02-18 17:04</t>
-  </si>
-  <si>
-    <t>2022-02-18 19:11</t>
-  </si>
-  <si>
-    <t>2022-02-18 16:59</t>
+    <t>2022-02-17 08:15</t>
+  </si>
+  <si>
+    <t>2022-02-17 08:08</t>
+  </si>
+  <si>
+    <t>2022-02-17 08:22</t>
+  </si>
+  <si>
+    <t>2022-02-17 07:23</t>
+  </si>
+  <si>
+    <t>2022-02-17 09:40</t>
+  </si>
+  <si>
+    <t>2022-02-17 06:05</t>
+  </si>
+  <si>
+    <t>2022-02-17 07:20</t>
+  </si>
+  <si>
+    <t>2022-02-17 11:58</t>
+  </si>
+  <si>
+    <t>2022-02-17 10:48</t>
+  </si>
+  <si>
+    <t>2022-02-17 11:11</t>
+  </si>
+  <si>
+    <t>2022-02-17 11:57</t>
+  </si>
+  <si>
+    <t>2022-02-17 12:21</t>
+  </si>
+  <si>
+    <t>2022-02-17 10:20</t>
+  </si>
+  <si>
+    <t>2022-02-17 10:57</t>
+  </si>
+  <si>
+    <t>2022-02-17 17:55</t>
+  </si>
+  <si>
+    <t>2022-02-17 18:20</t>
+  </si>
+  <si>
+    <t>2022-02-17 18:44</t>
+  </si>
+  <si>
+    <t>2022-02-17 18:48</t>
+  </si>
+  <si>
+    <t>2022-02-17 17:39</t>
+  </si>
+  <si>
+    <t>2022-02-17 17:47</t>
+  </si>
+  <si>
+    <t>2022-02-17 19:46</t>
+  </si>
+  <si>
+    <t>2022-02-18 07:44</t>
+  </si>
+  <si>
+    <t>2022-02-18 07:17</t>
+  </si>
+  <si>
+    <t>2022-02-18 06:41</t>
+  </si>
+  <si>
+    <t>2022-02-18 08:00</t>
+  </si>
+  <si>
+    <t>2022-02-18 08:19</t>
+  </si>
+  <si>
+    <t>2022-02-18 06:34</t>
+  </si>
+  <si>
+    <t>2022-02-18 08:09</t>
+  </si>
+  <si>
+    <t>2022-02-18 12:47</t>
+  </si>
+  <si>
+    <t>2022-02-18 12:55</t>
+  </si>
+  <si>
+    <t>2022-02-18 11:14</t>
+  </si>
+  <si>
+    <t>2022-02-18 12:01</t>
+  </si>
+  <si>
+    <t>2022-02-18 14:29</t>
+  </si>
+  <si>
+    <t>2022-02-18 12:05</t>
+  </si>
+  <si>
+    <t>2022-02-18 12:04</t>
+  </si>
+  <si>
+    <t>2022-02-18 17:05</t>
+  </si>
+  <si>
+    <t>2022-02-18 18:36</t>
+  </si>
+  <si>
+    <t>2022-02-18 18:37</t>
+  </si>
+  <si>
+    <t>2022-02-18 19:07</t>
+  </si>
+  <si>
+    <t>2022-02-18 18:26</t>
   </si>
   <si>
     <t>2022-02-18 18:53</t>
   </si>
   <si>
-    <t>2022-02-18 17:17</t>
-  </si>
-  <si>
-    <t>2022-02-18 18:24</t>
-  </si>
-  <si>
-    <t>2022-02-18 18:26</t>
-  </si>
-  <si>
-    <t>2022-02-19 07:28</t>
-  </si>
-  <si>
-    <t>2022-02-19 06:26</t>
-  </si>
-  <si>
-    <t>2022-02-19 06:19</t>
-  </si>
-  <si>
-    <t>2022-02-19 08:44</t>
-  </si>
-  <si>
-    <t>2022-02-19 08:12</t>
-  </si>
-  <si>
-    <t>2022-02-19 09:33</t>
-  </si>
-  <si>
-    <t>2022-02-19 07:19</t>
-  </si>
-  <si>
-    <t>2022-02-19 12:56</t>
-  </si>
-  <si>
-    <t>2022-02-19 11:55</t>
-  </si>
-  <si>
-    <t>2022-02-19 12:08</t>
+    <t>2022-02-18 17:47</t>
+  </si>
+  <si>
+    <t>2022-02-19 08:43</t>
+  </si>
+  <si>
+    <t>2022-02-19 08:50</t>
+  </si>
+  <si>
+    <t>2022-02-19 07:26</t>
+  </si>
+  <si>
+    <t>2022-02-19 06:38</t>
+  </si>
+  <si>
+    <t>2022-02-19 09:04</t>
+  </si>
+  <si>
+    <t>2022-02-19 08:08</t>
+  </si>
+  <si>
+    <t>2022-02-19 06:55</t>
+  </si>
+  <si>
+    <t>2022-02-19 12:20</t>
+  </si>
+  <si>
+    <t>2022-02-19 11:09</t>
+  </si>
+  <si>
+    <t>2022-02-19 12:13</t>
+  </si>
+  <si>
+    <t>2022-02-19 12:52</t>
+  </si>
+  <si>
+    <t>2022-02-19 12:21</t>
   </si>
   <si>
     <t>2022-02-19 12:50</t>
   </si>
   <si>
-    <t>2022-02-19 12:47</t>
-  </si>
-  <si>
-    <t>2022-02-19 12:52</t>
-  </si>
-  <si>
-    <t>2022-02-19 13:21</t>
-  </si>
-  <si>
-    <t>2022-02-19 16:58</t>
-  </si>
-  <si>
-    <t>2022-02-19 19:00</t>
-  </si>
-  <si>
-    <t>2022-02-19 17:23</t>
-  </si>
-  <si>
-    <t>2022-02-19 18:24</t>
-  </si>
-  <si>
-    <t>2022-02-19 17:02</t>
-  </si>
-  <si>
-    <t>2022-02-19 18:20</t>
-  </si>
-  <si>
-    <t>2022-02-19 16:55</t>
-  </si>
-  <si>
-    <t>2022-02-20 06:29</t>
-  </si>
-  <si>
-    <t>2022-02-20 07:55</t>
-  </si>
-  <si>
-    <t>2022-02-20 06:24</t>
-  </si>
-  <si>
-    <t>2022-02-20 08:33</t>
-  </si>
-  <si>
-    <t>2022-02-20 08:48</t>
-  </si>
-  <si>
-    <t>2022-02-20 07:18</t>
-  </si>
-  <si>
-    <t>2022-02-20 07:06</t>
-  </si>
-  <si>
-    <t>2022-02-20 13:15</t>
-  </si>
-  <si>
-    <t>2022-02-20 10:10</t>
-  </si>
-  <si>
-    <t>2022-02-20 11:29</t>
-  </si>
-  <si>
-    <t>2022-02-20 13:25</t>
-  </si>
-  <si>
-    <t>2022-02-20 10:36</t>
-  </si>
-  <si>
-    <t>2022-02-20 12:15</t>
-  </si>
-  <si>
-    <t>2022-02-20 11:26</t>
-  </si>
-  <si>
-    <t>2022-02-20 18:12</t>
-  </si>
-  <si>
-    <t>2022-02-20 18:10</t>
-  </si>
-  <si>
-    <t>2022-02-20 17:53</t>
-  </si>
-  <si>
-    <t>2022-02-20 17:33</t>
-  </si>
-  <si>
-    <t>2022-02-20 19:30</t>
-  </si>
-  <si>
-    <t>2022-02-20 17:58</t>
-  </si>
-  <si>
-    <t>2022-02-20 19:10</t>
-  </si>
-  <si>
-    <t>2022-02-21 07:12</t>
-  </si>
-  <si>
-    <t>2022-02-21 08:17</t>
-  </si>
-  <si>
-    <t>2022-02-21 09:57</t>
-  </si>
-  <si>
-    <t>2022-02-21 07:43</t>
-  </si>
-  <si>
-    <t>2022-02-21 07:57</t>
-  </si>
-  <si>
-    <t>2022-02-21 09:26</t>
-  </si>
-  <si>
-    <t>2022-02-21 09:00</t>
-  </si>
-  <si>
-    <t>2022-02-21 12:00</t>
-  </si>
-  <si>
-    <t>2022-02-21 12:06</t>
-  </si>
-  <si>
-    <t>2022-02-21 12:51</t>
-  </si>
-  <si>
-    <t>2022-02-21 13:30</t>
-  </si>
-  <si>
-    <t>2022-02-21 10:39</t>
-  </si>
-  <si>
-    <t>2022-02-21 11:03</t>
-  </si>
-  <si>
-    <t>2022-02-21 12:01</t>
-  </si>
-  <si>
-    <t>2022-02-21 18:24</t>
-  </si>
-  <si>
-    <t>2022-02-21 18:11</t>
-  </si>
-  <si>
-    <t>2022-02-21 17:47</t>
-  </si>
-  <si>
-    <t>2022-02-21 19:31</t>
-  </si>
-  <si>
-    <t>2022-02-21 18:05</t>
-  </si>
-  <si>
-    <t>2022-02-21 17:16</t>
+    <t>2022-02-19 11:26</t>
+  </si>
+  <si>
+    <t>2022-02-19 17:47</t>
+  </si>
+  <si>
+    <t>2022-02-19 15:56</t>
+  </si>
+  <si>
+    <t>2022-02-19 17:13</t>
+  </si>
+  <si>
+    <t>2022-02-19 19:07</t>
+  </si>
+  <si>
+    <t>2022-02-19 18:34</t>
+  </si>
+  <si>
+    <t>2022-02-19 18:12</t>
+  </si>
+  <si>
+    <t>2022-02-19 18:29</t>
+  </si>
+  <si>
+    <t>2022-02-20 07:02</t>
+  </si>
+  <si>
+    <t>2022-02-20 05:44</t>
+  </si>
+  <si>
+    <t>2022-02-20 08:58</t>
+  </si>
+  <si>
+    <t>2022-02-20 06:47</t>
+  </si>
+  <si>
+    <t>2022-02-20 08:30</t>
+  </si>
+  <si>
+    <t>2022-02-20 07:19</t>
+  </si>
+  <si>
+    <t>2022-02-20 05:49</t>
+  </si>
+  <si>
+    <t>2022-02-20 10:03</t>
+  </si>
+  <si>
+    <t>2022-02-20 11:46</t>
+  </si>
+  <si>
+    <t>2022-02-20 11:40</t>
+  </si>
+  <si>
+    <t>2022-02-20 12:07</t>
+  </si>
+  <si>
+    <t>2022-02-20 11:55</t>
+  </si>
+  <si>
+    <t>2022-02-20 13:19</t>
+  </si>
+  <si>
+    <t>2022-02-20 11:35</t>
+  </si>
+  <si>
+    <t>2022-02-20 17:26</t>
+  </si>
+  <si>
+    <t>2022-02-20 19:25</t>
+  </si>
+  <si>
+    <t>2022-02-20 17:11</t>
+  </si>
+  <si>
+    <t>2022-02-20 18:07</t>
+  </si>
+  <si>
+    <t>2022-02-20 18:59</t>
+  </si>
+  <si>
+    <t>2022-02-20 16:34</t>
+  </si>
+  <si>
+    <t>2022-02-20 17:49</t>
+  </si>
+  <si>
+    <t>2022-02-21 05:32</t>
+  </si>
+  <si>
+    <t>2022-02-21 08:16</t>
+  </si>
+  <si>
+    <t>2022-02-21 09:29</t>
+  </si>
+  <si>
+    <t>2022-02-21 08:51</t>
+  </si>
+  <si>
+    <t>2022-02-21 07:48</t>
+  </si>
+  <si>
+    <t>2022-02-21 08:37</t>
+  </si>
+  <si>
+    <t>2022-02-21 08:03</t>
+  </si>
+  <si>
+    <t>2022-02-21 11:26</t>
+  </si>
+  <si>
+    <t>2022-02-21 11:56</t>
+  </si>
+  <si>
+    <t>2022-02-21 11:25</t>
+  </si>
+  <si>
+    <t>2022-02-21 12:13</t>
+  </si>
+  <si>
+    <t>2022-02-21 10:29</t>
+  </si>
+  <si>
+    <t>2022-02-21 11:52</t>
+  </si>
+  <si>
+    <t>2022-02-21 12:32</t>
+  </si>
+  <si>
+    <t>2022-02-21 17:37</t>
+  </si>
+  <si>
+    <t>2022-02-21 17:27</t>
+  </si>
+  <si>
+    <t>2022-02-21 20:14</t>
+  </si>
+  <si>
+    <t>2022-02-21 16:39</t>
+  </si>
+  <si>
+    <t>2022-02-21 18:48</t>
+  </si>
+  <si>
+    <t>2022-02-21 16:33</t>
+  </si>
+  <si>
+    <t>2022-02-21 16:49</t>
   </si>
 </sst>
 </file>
@@ -786,13 +789,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="D2">
-        <v>0.9500000000000003</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -800,144 +803,144 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D3">
-        <v>0.8000000000000002</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>0.25</v>
       </c>
       <c r="D4">
-        <v>0.7500000000000001</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="D5">
-        <v>0.8000000000000002</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D7">
-        <v>0.8500000000000002</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>32</v>
       </c>
       <c r="C8">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D8">
-        <v>0.7500000000000001</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
       </c>
       <c r="C9">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D9">
-        <v>0.8000000000000002</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
       </c>
       <c r="C10">
-        <v>0.2</v>
+        <v>0.35</v>
       </c>
       <c r="D10">
-        <v>0.6</v>
+        <v>0.7500000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
         <v>35</v>
       </c>
       <c r="C11">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
       </c>
       <c r="C12">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
@@ -946,40 +949,40 @@
         <v>0.2</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
         <v>38</v>
       </c>
       <c r="C14">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D14">
-        <v>0.8500000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
         <v>39</v>
       </c>
       <c r="C15">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="D15">
-        <v>0.9500000000000003</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
         <v>40</v>
@@ -993,7 +996,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
         <v>41</v>
@@ -1002,12 +1005,12 @@
         <v>0.3</v>
       </c>
       <c r="D17">
-        <v>0.7000000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
         <v>42</v>
@@ -1016,12 +1019,12 @@
         <v>0.1</v>
       </c>
       <c r="D18">
-        <v>0.8500000000000002</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
         <v>43</v>
@@ -1035,7 +1038,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
         <v>44</v>
@@ -1044,32 +1047,32 @@
         <v>0.25</v>
       </c>
       <c r="D20">
-        <v>0.8000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
         <v>45</v>
       </c>
       <c r="C21">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
         <v>46</v>
       </c>
       <c r="C22">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="D22">
         <v>0.8000000000000002</v>
@@ -1077,49 +1080,49 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
         <v>47</v>
       </c>
       <c r="C23">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D23">
-        <v>0.7000000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
         <v>48</v>
       </c>
       <c r="C24">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="D24">
-        <v>0.9500000000000003</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
         <v>49</v>
       </c>
       <c r="C25">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="D25">
-        <v>0.8500000000000002</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
         <v>50</v>
@@ -1128,54 +1131,54 @@
         <v>0.05</v>
       </c>
       <c r="D26">
-        <v>0.8500000000000002</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
         <v>51</v>
       </c>
       <c r="C27">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D27">
-        <v>0.65</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
         <v>52</v>
       </c>
       <c r="C28">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="D28">
-        <v>0.8500000000000002</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
         <v>53</v>
       </c>
       <c r="C29">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D29">
-        <v>0.7500000000000001</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
         <v>54</v>
@@ -1184,40 +1187,40 @@
         <v>0.25</v>
       </c>
       <c r="D30">
-        <v>0.7500000000000001</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B31" t="s">
         <v>55</v>
       </c>
       <c r="C31">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="D31">
-        <v>0.8000000000000002</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B32" t="s">
         <v>56</v>
       </c>
       <c r="C32">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D32">
-        <v>0.8500000000000002</v>
+        <v>0.7500000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
         <v>57</v>
@@ -1226,40 +1229,40 @@
         <v>0.25</v>
       </c>
       <c r="D33">
-        <v>0.7000000000000001</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
         <v>58</v>
       </c>
       <c r="C34">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="D34">
-        <v>0.7500000000000001</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B35" t="s">
         <v>59</v>
       </c>
       <c r="C35">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D35">
-        <v>0.8000000000000002</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
         <v>60</v>
@@ -1268,40 +1271,40 @@
         <v>0.35</v>
       </c>
       <c r="D36">
-        <v>0.9000000000000002</v>
+        <v>0.7500000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B37" t="s">
         <v>61</v>
       </c>
       <c r="C37">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="D37">
-        <v>0.9500000000000003</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B38" t="s">
         <v>62</v>
       </c>
       <c r="C38">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="D38">
-        <v>0.9500000000000003</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B39" t="s">
         <v>63</v>
@@ -1315,13 +1318,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
         <v>64</v>
       </c>
       <c r="C40">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="D40">
         <v>0.9000000000000002</v>
@@ -1329,21 +1332,21 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B41" t="s">
         <v>65</v>
       </c>
       <c r="C41">
-        <v>0.45</v>
+        <v>0.25</v>
       </c>
       <c r="D41">
-        <v>0.8500000000000002</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B42" t="s">
         <v>66</v>
@@ -1352,376 +1355,376 @@
         <v>0.25</v>
       </c>
       <c r="D42">
-        <v>0.9000000000000002</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s">
         <v>67</v>
       </c>
       <c r="C43">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D43">
-        <v>0.7500000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B44" t="s">
         <v>68</v>
       </c>
       <c r="C44">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
       <c r="D44">
-        <v>0.9000000000000002</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B45" t="s">
         <v>69</v>
       </c>
       <c r="C45">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="D45">
-        <v>0.9500000000000003</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B46" t="s">
         <v>70</v>
       </c>
       <c r="C46">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="D46">
-        <v>0.8500000000000002</v>
+        <v>0.7500000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B47" t="s">
         <v>71</v>
       </c>
       <c r="C47">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B48" t="s">
         <v>72</v>
       </c>
       <c r="C48">
-        <v>0.2</v>
+        <v>0.35</v>
       </c>
       <c r="D48">
-        <v>0.8000000000000002</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B49" t="s">
         <v>73</v>
       </c>
       <c r="C49">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="D49">
-        <v>0.9500000000000003</v>
+        <v>0.7500000000000001</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B50" t="s">
         <v>74</v>
       </c>
       <c r="C50">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="D50">
-        <v>0.7500000000000001</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B51" t="s">
         <v>75</v>
       </c>
       <c r="C51">
-        <v>0.4</v>
+        <v>0.15</v>
       </c>
       <c r="D51">
-        <v>0.65</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B52" t="s">
         <v>76</v>
       </c>
       <c r="C52">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B53" t="s">
         <v>77</v>
       </c>
       <c r="C53">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="D53">
-        <v>0.7500000000000001</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B54" t="s">
         <v>78</v>
       </c>
       <c r="C54">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D54">
-        <v>0.9000000000000002</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B55" t="s">
         <v>79</v>
       </c>
       <c r="C55">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="D55">
-        <v>0.65</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B56" t="s">
         <v>80</v>
       </c>
       <c r="C56">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="D56">
-        <v>0.8000000000000002</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B57" t="s">
         <v>81</v>
       </c>
       <c r="C57">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="D57">
-        <v>0.7500000000000001</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B58" t="s">
         <v>82</v>
       </c>
       <c r="C58">
-        <v>0.4999999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="D58">
-        <v>0.65</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B59" t="s">
         <v>83</v>
       </c>
       <c r="C59">
-        <v>0.25</v>
+        <v>0.45</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B60" t="s">
         <v>84</v>
       </c>
       <c r="C60">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="D60">
-        <v>0.65</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B61" t="s">
         <v>85</v>
       </c>
       <c r="C61">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
       <c r="D61">
-        <v>0.7500000000000001</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B62" t="s">
         <v>86</v>
       </c>
       <c r="C62">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="D62">
-        <v>0.6</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B63" t="s">
         <v>87</v>
       </c>
       <c r="C63">
-        <v>0.25</v>
+        <v>0.4999999999999999</v>
       </c>
       <c r="D63">
-        <v>0.7500000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B64" t="s">
         <v>88</v>
       </c>
       <c r="C64">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="D64">
-        <v>0.9000000000000002</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B65" t="s">
         <v>89</v>
       </c>
       <c r="C65">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B66" t="s">
         <v>90</v>
       </c>
       <c r="C66">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B67" t="s">
         <v>91</v>
       </c>
       <c r="C67">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="D67">
-        <v>0.7000000000000001</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B68" t="s">
         <v>92</v>
       </c>
       <c r="C68">
-        <v>0.35</v>
+        <v>0.25</v>
       </c>
       <c r="D68">
-        <v>0.65</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B69" t="s">
         <v>93</v>
@@ -1730,7 +1733,7 @@
         <v>0.15</v>
       </c>
       <c r="D69">
-        <v>0.7500000000000001</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1741,21 +1744,21 @@
         <v>94</v>
       </c>
       <c r="C70">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D70">
-        <v>0.7000000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B71" t="s">
         <v>95</v>
       </c>
       <c r="C71">
-        <v>0.4</v>
+        <v>0.15</v>
       </c>
       <c r="D71">
         <v>0.9000000000000002</v>
@@ -1763,21 +1766,21 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B72" t="s">
         <v>96</v>
       </c>
       <c r="C72">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B73" t="s">
         <v>97</v>
@@ -1786,35 +1789,35 @@
         <v>0.25</v>
       </c>
       <c r="D73">
-        <v>0.7000000000000001</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B74" t="s">
         <v>98</v>
       </c>
       <c r="C74">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D74">
-        <v>0.7500000000000001</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B75" t="s">
         <v>99</v>
       </c>
       <c r="C75">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1825,15 +1828,15 @@
         <v>100</v>
       </c>
       <c r="C76">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="D76">
-        <v>0.8000000000000002</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B77" t="s">
         <v>101</v>
@@ -1842,12 +1845,12 @@
         <v>0.25</v>
       </c>
       <c r="D77">
-        <v>0.8000000000000002</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B78" t="s">
         <v>102</v>
@@ -1856,88 +1859,88 @@
         <v>0.25</v>
       </c>
       <c r="D78">
-        <v>0.8000000000000002</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B79" t="s">
         <v>103</v>
       </c>
       <c r="C79">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="D79">
-        <v>0.8500000000000002</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B80" t="s">
         <v>104</v>
       </c>
       <c r="C80">
-        <v>0.45</v>
+        <v>0.4</v>
       </c>
       <c r="D80">
-        <v>0.7500000000000001</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B81" t="s">
         <v>105</v>
       </c>
       <c r="C81">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B82" t="s">
         <v>106</v>
       </c>
       <c r="C82">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D82">
-        <v>0.7000000000000001</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B83" t="s">
         <v>107</v>
       </c>
       <c r="C83">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="D83">
-        <v>0.9000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B84" t="s">
         <v>108</v>
       </c>
       <c r="C84">
-        <v>0.25</v>
+        <v>0.45</v>
       </c>
       <c r="D84">
         <v>0.9500000000000003</v>
@@ -1945,21 +1948,21 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B85" t="s">
         <v>109</v>
       </c>
       <c r="C85">
-        <v>0.4999999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="D85">
-        <v>1</v>
+        <v>0.7500000000000001</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B86" t="s">
         <v>110</v>
@@ -1973,55 +1976,55 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B87" t="s">
         <v>111</v>
       </c>
       <c r="C87">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="D87">
-        <v>0.9000000000000002</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B88" t="s">
         <v>112</v>
       </c>
       <c r="C88">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D88">
-        <v>0.8500000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B89" t="s">
         <v>113</v>
       </c>
       <c r="C89">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D89">
-        <v>1</v>
+        <v>0.7500000000000001</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B90" t="s">
         <v>114</v>
       </c>
       <c r="C90">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="D90">
         <v>0.8500000000000002</v>
@@ -2029,7 +2032,7 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B91" t="s">
         <v>115</v>
@@ -2038,110 +2041,110 @@
         <v>0.35</v>
       </c>
       <c r="D91">
-        <v>0.65</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B92" t="s">
         <v>116</v>
       </c>
       <c r="C92">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="D92">
-        <v>0.8000000000000002</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B93" t="s">
         <v>117</v>
       </c>
       <c r="C93">
-        <v>0.4999999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="D93">
-        <v>0.9500000000000003</v>
+        <v>0.7500000000000001</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B94" t="s">
         <v>118</v>
       </c>
       <c r="C94">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="D94">
-        <v>0.8000000000000002</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B95" t="s">
         <v>119</v>
       </c>
       <c r="C95">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="D95">
-        <v>0.7000000000000001</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B96" t="s">
         <v>120</v>
       </c>
       <c r="C96">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="D96">
-        <v>0.8000000000000002</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B97" t="s">
         <v>121</v>
       </c>
       <c r="C97">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="D97">
-        <v>0.9000000000000002</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B98" t="s">
         <v>122</v>
       </c>
       <c r="C98">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="D98">
-        <v>0.7500000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B99" t="s">
         <v>123</v>
@@ -2150,18 +2153,18 @@
         <v>0.25</v>
       </c>
       <c r="D99">
-        <v>0.8000000000000002</v>
+        <v>0.9500000000000003</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B100" t="s">
         <v>124</v>
       </c>
       <c r="C100">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D100">
         <v>0.7500000000000001</v>
@@ -2169,69 +2172,69 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B101" t="s">
         <v>125</v>
       </c>
       <c r="C101">
-        <v>0.35</v>
+        <v>0.15</v>
       </c>
       <c r="D101">
-        <v>0.8000000000000002</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B102" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C102">
-        <v>0.1</v>
+        <v>0.35</v>
       </c>
       <c r="D102">
-        <v>0.8500000000000002</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B103" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C103">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="D103">
-        <v>0.9000000000000002</v>
+        <v>0.7500000000000001</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B104" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C104">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="D104">
-        <v>0.9000000000000002</v>
+        <v>0.8500000000000002</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B105" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C105">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="D105">
         <v>0.7500000000000001</v>
@@ -2239,16 +2242,16 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B106" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C106">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="D106">
-        <v>0.7500000000000001</v>
+        <v>0.9000000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>